<commit_message>
updated thinking7 hardware page with final node configuration
</commit_message>
<xml_diff>
--- a/source/leuven/tier2_hardware/thinking_hardware/thinking_node_map_v2_centos7.xlsx
+++ b/source/leuven/tier2_hardware/thinking_hardware/thinking_node_map_v2_centos7.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\HPC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\HPC\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -220,7 +220,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -296,18 +296,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor rgb="FFFF8080"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor rgb="FF800000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
         <bgColor rgb="FF800080"/>
       </patternFill>
     </fill>
@@ -318,7 +306,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -376,51 +364,6 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -493,7 +436,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -538,20 +481,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -626,6 +563,7 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
     <mruColors>
+      <color rgb="FF94070A"/>
       <color rgb="FFD99116"/>
     </mruColors>
   </colors>
@@ -909,7 +847,7 @@
   <dimension ref="A1:AA27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1042,43 +980,43 @@
       <c r="A5" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B5" s="26"/>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="40"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="26"/>
-      <c r="J5" s="26"/>
-      <c r="K5" s="26"/>
-      <c r="L5" s="26"/>
-      <c r="M5" s="26"/>
-      <c r="N5" s="26"/>
-      <c r="O5" s="26"/>
-      <c r="P5" s="26"/>
-      <c r="Q5" s="26"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
+      <c r="I5" s="28"/>
+      <c r="J5" s="28"/>
+      <c r="K5" s="28"/>
+      <c r="L5" s="28"/>
+      <c r="M5" s="28"/>
+      <c r="N5" s="28"/>
+      <c r="O5" s="28"/>
+      <c r="P5" s="28"/>
+      <c r="Q5" s="28"/>
     </row>
     <row r="6" spans="1:27" ht="13" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="26"/>
-      <c r="K6" s="26"/>
-      <c r="L6" s="26"/>
-      <c r="M6" s="26"/>
-      <c r="N6" s="26"/>
-      <c r="O6" s="26"/>
-      <c r="P6" s="26"/>
-      <c r="Q6" s="26"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="28"/>
+      <c r="J6" s="28"/>
+      <c r="K6" s="28"/>
+      <c r="L6" s="28"/>
+      <c r="M6" s="28"/>
+      <c r="N6" s="28"/>
+      <c r="O6" s="28"/>
+      <c r="P6" s="28"/>
+      <c r="Q6" s="28"/>
       <c r="U6" s="4" t="s">
         <v>7</v>
       </c>
@@ -1105,22 +1043,22 @@
       <c r="A7" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="40"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="26"/>
-      <c r="I7" s="26"/>
-      <c r="J7" s="26"/>
-      <c r="K7" s="26"/>
-      <c r="L7" s="26"/>
-      <c r="M7" s="26"/>
-      <c r="N7" s="26"/>
-      <c r="O7" s="26"/>
-      <c r="P7" s="26"/>
-      <c r="Q7" s="26"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="28"/>
+      <c r="J7" s="28"/>
+      <c r="K7" s="28"/>
+      <c r="L7" s="28"/>
+      <c r="M7" s="28"/>
+      <c r="N7" s="28"/>
+      <c r="O7" s="28"/>
+      <c r="P7" s="28"/>
+      <c r="Q7" s="28"/>
       <c r="S7" s="5"/>
       <c r="T7" s="6"/>
       <c r="U7" s="6" t="s">
@@ -1148,22 +1086,22 @@
       <c r="A8" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="26"/>
-      <c r="J8" s="26"/>
-      <c r="K8" s="26"/>
-      <c r="L8" s="26"/>
-      <c r="M8" s="26"/>
-      <c r="N8" s="40"/>
-      <c r="O8" s="26"/>
-      <c r="P8" s="26"/>
-      <c r="Q8" s="40"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="28"/>
+      <c r="J8" s="28"/>
+      <c r="K8" s="28"/>
+      <c r="L8" s="28"/>
+      <c r="M8" s="28"/>
+      <c r="N8" s="28"/>
+      <c r="O8" s="28"/>
+      <c r="P8" s="28"/>
+      <c r="Q8" s="28"/>
       <c r="S8" s="8"/>
       <c r="T8" s="9"/>
       <c r="U8" t="s">
@@ -1190,22 +1128,22 @@
       <c r="A9" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="27"/>
-      <c r="C9" s="27"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="41"/>
-      <c r="G9" s="41"/>
-      <c r="H9" s="27"/>
-      <c r="I9" s="27"/>
-      <c r="J9" s="41"/>
-      <c r="K9" s="41"/>
-      <c r="L9" s="41"/>
-      <c r="M9" s="27"/>
-      <c r="N9" s="27"/>
-      <c r="O9" s="27"/>
-      <c r="P9" s="27"/>
-      <c r="Q9" s="27"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="28"/>
+      <c r="I9" s="29"/>
+      <c r="J9" s="29"/>
+      <c r="K9" s="29"/>
+      <c r="L9" s="29"/>
+      <c r="M9" s="28"/>
+      <c r="N9" s="29"/>
+      <c r="O9" s="29"/>
+      <c r="P9" s="29"/>
+      <c r="Q9" s="29"/>
       <c r="S9" s="11"/>
       <c r="T9" s="6"/>
       <c r="U9" s="6" t="s">
@@ -1232,22 +1170,22 @@
       <c r="A10" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="41"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="27"/>
-      <c r="I10" s="27"/>
-      <c r="J10" s="27"/>
-      <c r="K10" s="27"/>
-      <c r="L10" s="27"/>
-      <c r="M10" s="27"/>
-      <c r="N10" s="27"/>
-      <c r="O10" s="27"/>
-      <c r="P10" s="27"/>
-      <c r="Q10" s="27"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="29"/>
+      <c r="I10" s="29"/>
+      <c r="J10" s="29"/>
+      <c r="K10" s="29"/>
+      <c r="L10" s="29"/>
+      <c r="M10" s="29"/>
+      <c r="N10" s="29"/>
+      <c r="O10" s="29"/>
+      <c r="P10" s="29"/>
+      <c r="Q10" s="29"/>
       <c r="S10" s="12"/>
       <c r="T10" s="9"/>
       <c r="U10" t="s">
@@ -1275,22 +1213,22 @@
       <c r="A11" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B11" s="26"/>
-      <c r="C11" s="26"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26"/>
-      <c r="H11" s="26"/>
-      <c r="I11" s="26"/>
-      <c r="J11" s="26"/>
-      <c r="K11" s="26"/>
-      <c r="L11" s="26"/>
-      <c r="M11" s="26"/>
-      <c r="N11" s="26"/>
-      <c r="O11" s="26"/>
-      <c r="P11" s="26"/>
-      <c r="Q11" s="26"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
+      <c r="I11" s="28"/>
+      <c r="J11" s="28"/>
+      <c r="K11" s="28"/>
+      <c r="L11" s="28"/>
+      <c r="M11" s="28"/>
+      <c r="N11" s="28"/>
+      <c r="O11" s="28"/>
+      <c r="P11" s="28"/>
+      <c r="Q11" s="28"/>
       <c r="S11" s="13"/>
       <c r="T11" s="6"/>
       <c r="U11" s="6" t="s">
@@ -1319,22 +1257,22 @@
       <c r="A12" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B12" s="26"/>
-      <c r="C12" s="26"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="26"/>
-      <c r="H12" s="26"/>
-      <c r="I12" s="26"/>
-      <c r="J12" s="26"/>
-      <c r="K12" s="26"/>
-      <c r="L12" s="26"/>
-      <c r="M12" s="26"/>
-      <c r="N12" s="26"/>
-      <c r="O12" s="26"/>
-      <c r="P12" s="26"/>
-      <c r="Q12" s="26"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="28"/>
+      <c r="J12" s="28"/>
+      <c r="K12" s="28"/>
+      <c r="L12" s="28"/>
+      <c r="M12" s="28"/>
+      <c r="N12" s="28"/>
+      <c r="O12" s="28"/>
+      <c r="P12" s="28"/>
+      <c r="Q12" s="28"/>
       <c r="S12" s="14"/>
       <c r="T12" s="9"/>
       <c r="U12" t="s">
@@ -1363,43 +1301,43 @@
       <c r="A13" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="27"/>
+      <c r="B13" s="16"/>
       <c r="C13" s="16"/>
       <c r="D13" s="16"/>
       <c r="E13" s="16"/>
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
-      <c r="H13" s="27"/>
-      <c r="I13" s="27"/>
-      <c r="J13" s="27"/>
-      <c r="K13" s="27"/>
-      <c r="L13" s="27"/>
-      <c r="M13" s="27"/>
-      <c r="N13" s="27"/>
-      <c r="O13" s="27"/>
-      <c r="P13" s="27"/>
-      <c r="Q13" s="27"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="16"/>
+      <c r="L13" s="16"/>
+      <c r="M13" s="16"/>
+      <c r="N13" s="16"/>
+      <c r="O13" s="16"/>
+      <c r="P13" s="16"/>
+      <c r="Q13" s="16"/>
     </row>
     <row r="14" spans="1:27" ht="13" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B14" s="26"/>
-      <c r="C14" s="26"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="26"/>
-      <c r="H14" s="26"/>
-      <c r="I14" s="26"/>
-      <c r="J14" s="26"/>
-      <c r="K14" s="26"/>
-      <c r="L14" s="26"/>
-      <c r="M14" s="26"/>
-      <c r="N14" s="26"/>
-      <c r="O14" s="26"/>
-      <c r="P14" s="26"/>
-      <c r="Q14" s="26"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="28"/>
+      <c r="J14" s="28"/>
+      <c r="K14" s="28"/>
+      <c r="L14" s="28"/>
+      <c r="M14" s="28"/>
+      <c r="N14" s="28"/>
+      <c r="O14" s="28"/>
+      <c r="P14" s="28"/>
+      <c r="Q14" s="28"/>
       <c r="X14" s="15" t="s">
         <v>21</v>
       </c>
@@ -1412,43 +1350,43 @@
       <c r="A15" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B15" s="26"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="26"/>
-      <c r="I15" s="26"/>
-      <c r="J15" s="26"/>
-      <c r="K15" s="26"/>
-      <c r="L15" s="26"/>
-      <c r="M15" s="26"/>
-      <c r="N15" s="26"/>
-      <c r="O15" s="26"/>
-      <c r="P15" s="26"/>
-      <c r="Q15" s="26"/>
-    </row>
-    <row r="16" spans="1:27" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="28"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="28"/>
+      <c r="J15" s="28"/>
+      <c r="K15" s="28"/>
+      <c r="L15" s="28"/>
+      <c r="M15" s="17"/>
+      <c r="N15" s="28"/>
+      <c r="O15" s="28"/>
+      <c r="P15" s="17"/>
+      <c r="Q15" s="17"/>
+    </row>
+    <row r="16" spans="1:27" ht="13" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B16" s="28"/>
+      <c r="B16" s="24"/>
       <c r="C16" s="24"/>
       <c r="D16" s="24"/>
       <c r="E16" s="24"/>
       <c r="F16" s="24"/>
       <c r="G16" s="24"/>
-      <c r="H16" s="28"/>
-      <c r="I16" s="28"/>
-      <c r="J16" s="28"/>
-      <c r="K16" s="28"/>
-      <c r="L16" s="28"/>
-      <c r="M16" s="28"/>
-      <c r="N16" s="28"/>
-      <c r="O16" s="28"/>
-      <c r="P16" s="28"/>
-      <c r="Q16" s="28"/>
+      <c r="H16" s="24"/>
+      <c r="I16" s="24"/>
+      <c r="J16" s="24"/>
+      <c r="K16" s="24"/>
+      <c r="L16" s="24"/>
+      <c r="M16" s="24"/>
+      <c r="N16" s="24"/>
+      <c r="O16" s="24"/>
+      <c r="P16" s="24"/>
+      <c r="Q16" s="24"/>
       <c r="S16" s="17"/>
       <c r="U16" t="s">
         <v>23</v>
@@ -1458,85 +1396,85 @@
       <c r="A17" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B17" s="29"/>
-      <c r="C17" s="30"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="30"/>
-      <c r="G17" s="30"/>
-      <c r="H17" s="30"/>
-      <c r="I17" s="30"/>
-      <c r="J17" s="30"/>
-      <c r="K17" s="30"/>
-      <c r="L17" s="30"/>
-      <c r="M17" s="30"/>
-      <c r="N17" s="30"/>
-      <c r="O17" s="30"/>
-      <c r="P17" s="30"/>
-      <c r="Q17" s="31"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="24"/>
+      <c r="I17" s="24"/>
+      <c r="J17" s="24"/>
+      <c r="K17" s="24"/>
+      <c r="L17" s="24"/>
+      <c r="M17" s="24"/>
+      <c r="N17" s="24"/>
+      <c r="O17" s="24"/>
+      <c r="P17" s="24"/>
+      <c r="Q17" s="24"/>
     </row>
     <row r="18" spans="1:21" ht="13" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B18" s="32"/>
-      <c r="C18" s="33"/>
-      <c r="D18" s="33"/>
-      <c r="E18" s="33"/>
-      <c r="F18" s="33"/>
-      <c r="G18" s="33"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="33"/>
-      <c r="J18" s="33"/>
-      <c r="K18" s="33"/>
-      <c r="L18" s="33"/>
-      <c r="M18" s="33"/>
-      <c r="N18" s="33"/>
-      <c r="O18" s="33"/>
-      <c r="P18" s="33"/>
-      <c r="Q18" s="34"/>
+      <c r="B18" s="30"/>
+      <c r="C18" s="31"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="31"/>
+      <c r="G18" s="31"/>
+      <c r="H18" s="31"/>
+      <c r="I18" s="31"/>
+      <c r="J18" s="31"/>
+      <c r="K18" s="31"/>
+      <c r="L18" s="31"/>
+      <c r="M18" s="31"/>
+      <c r="N18" s="31"/>
+      <c r="O18" s="31"/>
+      <c r="P18" s="31"/>
+      <c r="Q18" s="32"/>
     </row>
     <row r="19" spans="1:21" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="32"/>
-      <c r="C19" s="33"/>
-      <c r="D19" s="33"/>
-      <c r="E19" s="33"/>
-      <c r="F19" s="33"/>
-      <c r="G19" s="33"/>
-      <c r="H19" s="33"/>
-      <c r="I19" s="33"/>
-      <c r="J19" s="33"/>
-      <c r="K19" s="33"/>
-      <c r="L19" s="33"/>
-      <c r="M19" s="33"/>
-      <c r="N19" s="33"/>
-      <c r="O19" s="33"/>
-      <c r="P19" s="33"/>
-      <c r="Q19" s="34"/>
+      <c r="B19" s="30"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="31"/>
+      <c r="E19" s="31"/>
+      <c r="F19" s="31"/>
+      <c r="G19" s="31"/>
+      <c r="H19" s="31"/>
+      <c r="I19" s="31"/>
+      <c r="J19" s="31"/>
+      <c r="K19" s="31"/>
+      <c r="L19" s="31"/>
+      <c r="M19" s="31"/>
+      <c r="N19" s="31"/>
+      <c r="O19" s="31"/>
+      <c r="P19" s="31"/>
+      <c r="Q19" s="32"/>
     </row>
     <row r="20" spans="1:21" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B20" s="32"/>
-      <c r="C20" s="33"/>
-      <c r="D20" s="33"/>
-      <c r="E20" s="33"/>
-      <c r="F20" s="33"/>
-      <c r="G20" s="33"/>
-      <c r="H20" s="33"/>
-      <c r="I20" s="33"/>
-      <c r="J20" s="33"/>
-      <c r="K20" s="33"/>
-      <c r="L20" s="33"/>
-      <c r="M20" s="33"/>
-      <c r="N20" s="33"/>
-      <c r="O20" s="33"/>
-      <c r="P20" s="33"/>
-      <c r="Q20" s="34"/>
+      <c r="B20" s="30"/>
+      <c r="C20" s="31"/>
+      <c r="D20" s="31"/>
+      <c r="E20" s="31"/>
+      <c r="F20" s="31"/>
+      <c r="G20" s="31"/>
+      <c r="H20" s="31"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="31"/>
+      <c r="K20" s="31"/>
+      <c r="L20" s="31"/>
+      <c r="M20" s="31"/>
+      <c r="N20" s="31"/>
+      <c r="O20" s="31"/>
+      <c r="P20" s="31"/>
+      <c r="Q20" s="32"/>
       <c r="S20" s="25"/>
       <c r="U20" t="s">
         <v>24</v>
@@ -1546,22 +1484,22 @@
       <c r="A21" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B21" s="32"/>
-      <c r="C21" s="33"/>
-      <c r="D21" s="33"/>
-      <c r="E21" s="33"/>
-      <c r="F21" s="33"/>
-      <c r="G21" s="33"/>
-      <c r="H21" s="33"/>
-      <c r="I21" s="33"/>
-      <c r="J21" s="33"/>
-      <c r="K21" s="33"/>
-      <c r="L21" s="33"/>
-      <c r="M21" s="33"/>
-      <c r="N21" s="33"/>
-      <c r="O21" s="33"/>
-      <c r="P21" s="33"/>
-      <c r="Q21" s="34"/>
+      <c r="B21" s="30"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="31"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="31"/>
+      <c r="G21" s="31"/>
+      <c r="H21" s="31"/>
+      <c r="I21" s="31"/>
+      <c r="J21" s="31"/>
+      <c r="K21" s="31"/>
+      <c r="L21" s="31"/>
+      <c r="M21" s="31"/>
+      <c r="N21" s="31"/>
+      <c r="O21" s="31"/>
+      <c r="P21" s="31"/>
+      <c r="Q21" s="32"/>
       <c r="U21" t="s">
         <v>25</v>
       </c>
@@ -1570,43 +1508,43 @@
       <c r="A22" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B22" s="32"/>
-      <c r="C22" s="33"/>
-      <c r="D22" s="33"/>
-      <c r="E22" s="33"/>
-      <c r="F22" s="33"/>
-      <c r="G22" s="33"/>
-      <c r="H22" s="33"/>
-      <c r="I22" s="33"/>
-      <c r="J22" s="33"/>
-      <c r="K22" s="33"/>
-      <c r="L22" s="33"/>
-      <c r="M22" s="33"/>
-      <c r="N22" s="33"/>
-      <c r="O22" s="33"/>
-      <c r="P22" s="33"/>
-      <c r="Q22" s="34"/>
+      <c r="B22" s="30"/>
+      <c r="C22" s="31"/>
+      <c r="D22" s="31"/>
+      <c r="E22" s="31"/>
+      <c r="F22" s="31"/>
+      <c r="G22" s="31"/>
+      <c r="H22" s="31"/>
+      <c r="I22" s="31"/>
+      <c r="J22" s="31"/>
+      <c r="K22" s="31"/>
+      <c r="L22" s="31"/>
+      <c r="M22" s="31"/>
+      <c r="N22" s="31"/>
+      <c r="O22" s="31"/>
+      <c r="P22" s="31"/>
+      <c r="Q22" s="32"/>
     </row>
     <row r="23" spans="1:21" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>56</v>
       </c>
       <c r="B23" s="35"/>
-      <c r="C23" s="36"/>
-      <c r="D23" s="36"/>
-      <c r="E23" s="36"/>
-      <c r="F23" s="36"/>
-      <c r="G23" s="36"/>
-      <c r="H23" s="36"/>
-      <c r="I23" s="36"/>
-      <c r="J23" s="36"/>
-      <c r="K23" s="36"/>
-      <c r="L23" s="36"/>
-      <c r="M23" s="36"/>
-      <c r="N23" s="36"/>
-      <c r="O23" s="36"/>
-      <c r="P23" s="36"/>
-      <c r="Q23" s="37"/>
+      <c r="C23" s="33"/>
+      <c r="D23" s="33"/>
+      <c r="E23" s="33"/>
+      <c r="F23" s="33"/>
+      <c r="G23" s="33"/>
+      <c r="H23" s="33"/>
+      <c r="I23" s="33"/>
+      <c r="J23" s="33"/>
+      <c r="K23" s="33"/>
+      <c r="L23" s="33"/>
+      <c r="M23" s="33"/>
+      <c r="N23" s="33"/>
+      <c r="O23" s="33"/>
+      <c r="P23" s="33"/>
+      <c r="Q23" s="34"/>
     </row>
     <row r="24" spans="1:21" ht="13" x14ac:dyDescent="0.3">
       <c r="A24" s="21"/>
@@ -1666,13 +1604,13 @@
       </c>
       <c r="B26"/>
       <c r="C26"/>
-      <c r="D26" s="38"/>
-      <c r="E26" s="38"/>
-      <c r="F26" s="39"/>
-      <c r="G26" s="39"/>
-      <c r="H26" s="39"/>
-      <c r="I26" s="39"/>
-      <c r="J26" s="39"/>
+      <c r="D26" s="27"/>
+      <c r="E26" s="27"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="13"/>
+      <c r="I26" s="13"/>
+      <c r="J26" s="13"/>
       <c r="K26" s="20"/>
       <c r="L26" s="20"/>
       <c r="M26" s="20"/>

</xml_diff>

<commit_message>
Update node map issue #155
</commit_message>
<xml_diff>
--- a/source/leuven/tier2_hardware/thinking_hardware/thinking_node_map_v2_centos7.xlsx
+++ b/source/leuven/tier2_hardware/thinking_hardware/thinking_node_map_v2_centos7.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\geert\Documents\Data\Projects\VSC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\GitHub\VscDocumentation\source\leuven\tier2_hardware\thinking_hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32979A0C-AB76-49AA-886B-D1F4246DF9D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66BE2CE8-329F-42E9-885E-D3AAE341B92A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1065" yWindow="-120" windowWidth="27855" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="41">
   <si>
     <t>n10</t>
   </si>
@@ -87,9 +87,6 @@
     <t>E5-2650 v3</t>
   </si>
   <si>
-    <t>Quadro K5200</t>
-  </si>
-  <si>
     <t>total nodes</t>
   </si>
   <si>
@@ -132,19 +129,7 @@
     <t>n09</t>
   </si>
   <si>
-    <t>r04i00</t>
-  </si>
-  <si>
-    <t>r04i01</t>
-  </si>
-  <si>
     <t>r04i02</t>
-  </si>
-  <si>
-    <t>r05i00</t>
-  </si>
-  <si>
-    <t>r05i01</t>
   </si>
   <si>
     <t>r05i02</t>
@@ -200,7 +185,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -239,30 +224,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor rgb="FFFFFF00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor rgb="FFFF8080"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor rgb="FF800000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor rgb="FFFF8080"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor rgb="FF800000"/>
       </patternFill>
@@ -275,25 +236,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor theme="7" tint="-0.499984740745262"/>
         <bgColor rgb="FFFF8080"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
-        <bgColor rgb="FF800080"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
-        <bgColor rgb="FF008080"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="-0.499984740745262"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFFF8080"/>
       </patternFill>
     </fill>
@@ -473,7 +422,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -508,27 +457,26 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -880,10 +828,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AA18"/>
+  <dimension ref="A1:AC14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S11" sqref="S11"/>
+      <selection activeCell="Z5" sqref="Z5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -899,33 +847,33 @@
     <col min="28" max="1025" width="11.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
       <c r="B1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>0</v>
@@ -949,246 +897,233 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="32"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="32"/>
+      <c r="P2" s="32"/>
+      <c r="Q2" s="32"/>
+      <c r="T2" s="18"/>
+      <c r="V2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="W2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="X2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB2" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18"/>
-      <c r="M2" s="18"/>
-      <c r="N2" s="18"/>
-      <c r="O2" s="18"/>
-      <c r="P2" s="18"/>
-      <c r="Q2" s="18"/>
-      <c r="S2" s="22"/>
-      <c r="U2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="V2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="W2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="X2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="Y2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="Z2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="AA2" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="B3" s="34"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="34"/>
+      <c r="J3" s="34"/>
+      <c r="K3" s="34"/>
+      <c r="L3" s="34"/>
+      <c r="M3" s="34"/>
+      <c r="N3" s="34"/>
+      <c r="O3" s="34"/>
+      <c r="P3" s="34"/>
+      <c r="Q3" s="34"/>
+      <c r="T3" s="33"/>
+      <c r="U3" s="5"/>
+      <c r="V3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="W3" s="5">
+        <v>24</v>
+      </c>
+      <c r="X3" s="5">
+        <v>64</v>
+      </c>
+      <c r="Y3" s="6"/>
+      <c r="Z3" s="6">
+        <v>36</v>
+      </c>
+      <c r="AA3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB3" s="5">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-      <c r="K3" s="18"/>
-      <c r="L3" s="18"/>
-      <c r="M3" s="18"/>
-      <c r="N3" s="18"/>
-      <c r="O3" s="18"/>
-      <c r="P3" s="18"/>
-      <c r="Q3" s="18"/>
-      <c r="S3" s="21"/>
-      <c r="T3" s="5"/>
-      <c r="U3" s="5" t="s">
+      <c r="B4" s="35"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="36"/>
+      <c r="J4" s="36"/>
+      <c r="K4" s="36"/>
+      <c r="L4" s="36"/>
+      <c r="M4" s="36"/>
+      <c r="N4" s="36"/>
+      <c r="O4" s="36"/>
+      <c r="P4" s="36"/>
+      <c r="Q4" s="37"/>
+      <c r="T4" s="19"/>
+      <c r="U4" s="7"/>
+      <c r="V4" t="s">
         <v>14</v>
       </c>
-      <c r="V3" s="5">
+      <c r="W4">
         <v>24</v>
       </c>
-      <c r="W3" s="5">
+      <c r="X4">
+        <v>128</v>
+      </c>
+      <c r="Y4" s="8"/>
+      <c r="Z4" s="8">
+        <v>72</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB4">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="25"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="26"/>
+      <c r="M5" s="26"/>
+      <c r="N5" s="26"/>
+      <c r="O5" s="26"/>
+      <c r="P5" s="26"/>
+      <c r="Q5" s="27"/>
+      <c r="T5" s="20"/>
+      <c r="U5" s="5"/>
+      <c r="V5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="W5" s="5">
+        <v>20</v>
+      </c>
+      <c r="X5" s="5">
         <v>64</v>
       </c>
-      <c r="X3" s="6"/>
-      <c r="Y3" s="6">
-        <v>48</v>
-      </c>
-      <c r="Z3" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="AA3" s="5">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="19"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19"/>
-      <c r="J4" s="19"/>
-      <c r="K4" s="19"/>
-      <c r="L4" s="19"/>
-      <c r="M4" s="19"/>
-      <c r="N4" s="19"/>
-      <c r="O4" s="19"/>
-      <c r="P4" s="19"/>
-      <c r="Q4" s="19"/>
-      <c r="S4" s="23"/>
-      <c r="T4" s="7"/>
-      <c r="U4" t="s">
-        <v>14</v>
-      </c>
-      <c r="V4">
-        <v>24</v>
-      </c>
-      <c r="W4">
-        <v>128</v>
-      </c>
-      <c r="X4" s="8"/>
-      <c r="Y4" s="8">
-        <f>6*16</f>
-        <v>96</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>15</v>
-      </c>
-      <c r="AA4">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+      <c r="Y5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z5" s="6">
+        <v>5</v>
+      </c>
+      <c r="AA5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB5" s="5">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="18"/>
-      <c r="L5" s="18"/>
-      <c r="M5" s="18"/>
-      <c r="N5" s="18"/>
-      <c r="O5" s="18"/>
-      <c r="P5" s="18"/>
-      <c r="Q5" s="18"/>
-      <c r="S5" s="24"/>
-      <c r="T5" s="5"/>
-      <c r="U5" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="V5" s="5">
-        <v>20</v>
-      </c>
-      <c r="W5" s="5">
-        <v>64</v>
-      </c>
-      <c r="X5" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="Y5" s="6">
-        <v>5</v>
-      </c>
-      <c r="Z5" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="AA5" s="5">
-        <v>2.2999999999999998</v>
-      </c>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+      <c r="B6" s="25"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="26"/>
+      <c r="J6" s="26"/>
+      <c r="K6" s="26"/>
+      <c r="L6" s="26"/>
+      <c r="M6" s="26"/>
+      <c r="N6" s="26"/>
+      <c r="O6" s="26"/>
+      <c r="P6" s="26"/>
+      <c r="Q6" s="27"/>
+      <c r="T6" s="24"/>
+      <c r="U6" s="7"/>
+      <c r="Y6" s="8"/>
+      <c r="Z6" s="8"/>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="18"/>
-      <c r="M6" s="18"/>
-      <c r="N6" s="18"/>
-      <c r="O6" s="18"/>
-      <c r="P6" s="18"/>
-      <c r="Q6" s="18"/>
-      <c r="S6" s="34"/>
-      <c r="T6" s="7"/>
-      <c r="U6" t="s">
-        <v>14</v>
-      </c>
-      <c r="V6">
-        <v>20</v>
-      </c>
-      <c r="W6">
-        <v>128</v>
-      </c>
-      <c r="X6" s="8" t="s">
+      <c r="B7" s="25"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
+      <c r="I7" s="26"/>
+      <c r="J7" s="26"/>
+      <c r="K7" s="26"/>
+      <c r="L7" s="26"/>
+      <c r="M7" s="26"/>
+      <c r="N7" s="26"/>
+      <c r="O7" s="26"/>
+      <c r="P7" s="26"/>
+      <c r="Q7" s="27"/>
+      <c r="Y7" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="Y6" s="8">
-        <v>2</v>
-      </c>
-      <c r="Z6" t="s">
-        <v>17</v>
-      </c>
-      <c r="AA6">
-        <v>2.2999999999999998</v>
-      </c>
-    </row>
-    <row r="7" spans="1:27" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="Z7">
+        <f>SUM(Z3:Z6)</f>
+        <v>113</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="B7" s="20"/>
-      <c r="C7" s="38"/>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
-      <c r="F7" s="38"/>
-      <c r="G7" s="38"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="20"/>
-      <c r="K7" s="20"/>
-      <c r="L7" s="20"/>
-      <c r="M7" s="20"/>
-      <c r="N7" s="20"/>
-      <c r="O7" s="20"/>
-      <c r="P7" s="20"/>
-      <c r="Q7" s="20"/>
-    </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>39</v>
       </c>
       <c r="B8" s="25"/>
       <c r="C8" s="26"/>
@@ -1205,232 +1140,146 @@
       <c r="N8" s="26"/>
       <c r="O8" s="26"/>
       <c r="P8" s="26"/>
-      <c r="Q8" s="31"/>
-      <c r="X8" s="9" t="s">
+      <c r="Q8" s="27"/>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="25"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="26"/>
+      <c r="J9" s="26"/>
+      <c r="K9" s="26"/>
+      <c r="L9" s="26"/>
+      <c r="M9" s="26"/>
+      <c r="N9" s="26"/>
+      <c r="O9" s="26"/>
+      <c r="P9" s="26"/>
+      <c r="Q9" s="27"/>
+      <c r="T9" s="10"/>
+      <c r="V9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" s="28"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="29"/>
+      <c r="I10" s="29"/>
+      <c r="J10" s="29"/>
+      <c r="K10" s="29"/>
+      <c r="L10" s="29"/>
+      <c r="M10" s="29"/>
+      <c r="N10" s="29"/>
+      <c r="O10" s="29"/>
+      <c r="P10" s="29"/>
+      <c r="Q10" s="30"/>
+    </row>
+    <row r="11" spans="1:29" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="14"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="11"/>
+      <c r="O11" s="11"/>
+      <c r="P11" s="11"/>
+      <c r="Q11" s="11"/>
+      <c r="R11" s="12"/>
+      <c r="T11" s="17"/>
+      <c r="V11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A12" s="3"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="13"/>
+      <c r="N12" s="15"/>
+      <c r="O12" s="15"/>
+      <c r="P12" s="15"/>
+      <c r="Q12" s="15"/>
+      <c r="R12" s="16"/>
+      <c r="V12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="Y8">
-        <f>SUM(Y3:Y6)</f>
-        <v>151</v>
-      </c>
-    </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B9" s="27"/>
-      <c r="C9" s="28"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="28"/>
-      <c r="I9" s="28"/>
-      <c r="J9" s="28"/>
-      <c r="K9" s="28"/>
-      <c r="L9" s="28"/>
-      <c r="M9" s="28"/>
-      <c r="N9" s="28"/>
-      <c r="O9" s="28"/>
-      <c r="P9" s="28"/>
-      <c r="Q9" s="32"/>
-    </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B10" s="27"/>
-      <c r="C10" s="28"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="28"/>
-      <c r="H10" s="28"/>
-      <c r="I10" s="28"/>
-      <c r="J10" s="28"/>
-      <c r="K10" s="28"/>
-      <c r="L10" s="28"/>
-      <c r="M10" s="28"/>
-      <c r="N10" s="28"/>
-      <c r="O10" s="28"/>
-      <c r="P10" s="28"/>
-      <c r="Q10" s="32"/>
-    </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B11" s="27"/>
-      <c r="C11" s="28"/>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="28"/>
-      <c r="I11" s="28"/>
-      <c r="J11" s="28"/>
-      <c r="K11" s="28"/>
-      <c r="L11" s="28"/>
-      <c r="M11" s="28"/>
-      <c r="N11" s="28"/>
-      <c r="O11" s="28"/>
-      <c r="P11" s="28"/>
-      <c r="Q11" s="32"/>
-      <c r="S11" s="10"/>
-      <c r="U11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:27" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B12" s="27"/>
-      <c r="C12" s="28"/>
-      <c r="D12" s="28"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="28"/>
-      <c r="G12" s="28"/>
-      <c r="H12" s="28"/>
-      <c r="I12" s="28"/>
-      <c r="J12" s="28"/>
-      <c r="K12" s="28"/>
-      <c r="L12" s="28"/>
-      <c r="M12" s="28"/>
-      <c r="N12" s="28"/>
-      <c r="O12" s="28"/>
-      <c r="P12" s="28"/>
-      <c r="Q12" s="32"/>
-    </row>
-    <row r="13" spans="1:27" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B13" s="27"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="28"/>
-      <c r="G13" s="28"/>
-      <c r="H13" s="28"/>
-      <c r="I13" s="28"/>
-      <c r="J13" s="28"/>
-      <c r="K13" s="28"/>
-      <c r="L13" s="28"/>
-      <c r="M13" s="28"/>
-      <c r="N13" s="28"/>
-      <c r="O13" s="28"/>
-      <c r="P13" s="28"/>
-      <c r="Q13" s="32"/>
-      <c r="S13" s="17"/>
-      <c r="U13" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:27" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B14" s="29"/>
-      <c r="C14" s="30"/>
-      <c r="D14" s="30"/>
-      <c r="E14" s="30"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="30"/>
-      <c r="H14" s="30"/>
-      <c r="I14" s="30"/>
-      <c r="J14" s="30"/>
-      <c r="K14" s="30"/>
-      <c r="L14" s="30"/>
-      <c r="M14" s="30"/>
-      <c r="N14" s="30"/>
-      <c r="O14" s="30"/>
-      <c r="P14" s="30"/>
-      <c r="Q14" s="33"/>
-      <c r="U14" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A15" s="14"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="12"/>
-      <c r="K15" s="12"/>
-      <c r="L15" s="12"/>
-      <c r="M15" s="12"/>
-      <c r="N15" s="11"/>
-      <c r="O15" s="11"/>
-      <c r="P15" s="11"/>
-      <c r="Q15" s="11"/>
-      <c r="R15" s="12"/>
-    </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A16" s="3"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="K16" s="13"/>
-      <c r="L16" s="13"/>
-      <c r="M16" s="13"/>
-      <c r="N16" s="15"/>
-      <c r="O16" s="15"/>
-      <c r="P16" s="15"/>
-      <c r="Q16" s="15"/>
-      <c r="R16" s="16"/>
-    </row>
-    <row r="17" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17"/>
-      <c r="C17"/>
-      <c r="D17" s="36"/>
-      <c r="E17" s="36"/>
-      <c r="F17" s="35"/>
-      <c r="G17" s="35"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="35"/>
-      <c r="K17" s="13"/>
-      <c r="L17" s="13"/>
-      <c r="M17" s="13"/>
-      <c r="N17" s="15"/>
-      <c r="O17" s="15"/>
-      <c r="P17" s="15"/>
-      <c r="Q17" s="15"/>
-      <c r="R17" s="16"/>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="K18" s="7"/>
-      <c r="L18" s="7"/>
-      <c r="M18" s="7"/>
-      <c r="N18" s="7"/>
-      <c r="O18" s="7"/>
-      <c r="P18" s="7"/>
-      <c r="Q18" s="7"/>
+      <c r="B13"/>
+      <c r="C13"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="31"/>
+      <c r="G13" s="31"/>
+      <c r="H13" s="31"/>
+      <c r="I13" s="31"/>
+      <c r="J13" s="31"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
+      <c r="M13" s="13"/>
+      <c r="N13" s="15"/>
+      <c r="O13" s="15"/>
+      <c r="P13" s="15"/>
+      <c r="Q13" s="15"/>
+      <c r="R13" s="16"/>
+      <c r="Y13"/>
+      <c r="Z13"/>
+      <c r="AA13"/>
+      <c r="AB13"/>
+      <c r="AC13"/>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="7"/>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.78740157480314965" right="0.78740157480314965" top="1.0629921259842521" bottom="1.0629921259842521" header="0.78740157480314965" footer="0.78740157480314965"/>

</xml_diff>